<commit_message>
Neue Dokumente, Kanban Beschrieb, StatusBericht Template
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Datum</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Aufsetzen eigener Branch in RCS, Workspace einrichten, Testen</t>
+  </si>
+  <si>
+    <t>Vorbereiten Präsentationstechnikkurs</t>
+  </si>
+  <si>
+    <t>Feedback aus Kickoff verarbeiten</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,25 +524,47 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>41399</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>41400</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>41400</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="4">
-        <f>SUM(C2:C34)</f>
-        <v>34</v>
+      <c r="C34" s="4">
+        <f>SUM(C2:C33)</f>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weitergefahren mit dem Projektantrag
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -54,7 +54,8 @@
     <t>Feedback aus Kickoff verarbeiten</t>
   </si>
   <si>
-    <t>Abstract und Projektantrag erarbeiten</t>
+    <t>Abstract und Projektantrag erarbeiten, Logo-/Bildsuche für Arbeit
+Templates vorbereiten</t>
   </si>
 </sst>
 </file>
@@ -119,12 +120,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -429,7 +436,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="A13:B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,15 +567,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>41403</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -578,7 +585,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abstract angepasst, Kickoff Fragen und Antworten dokumentiert, Planung und TODOS angepasst, neue Icons
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Theorie Migration E3 to E4 durchgelesen</t>
+  </si>
+  <si>
+    <t>Überarbeitung Projektantrag</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +610,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>41409</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
@@ -614,7 +628,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diverse Planungs-Dokumente aktualisiert, Vorlage Aspektmigration
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Projektantrag, Risiken etc</t>
+  </si>
+  <si>
+    <t>Projektantrag, Risiken etc, Evaluation welche Aspekte es gibt</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,6 +652,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>41414</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1">
+        <v>8</v>
+      </c>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
@@ -656,7 +670,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weitergefahren mit möglichen Aspekte, Planung angepasst, Migrationsmöglichkeiten angeschaut
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12600" windowHeight="12405"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Datum</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Ideen für Aspekte sammeln (in RCS, und sonst e3)</t>
+  </si>
+  <si>
+    <t>Besprechung mit Betreuer, Planung anpassen, Versuche mit E3 E4 Mix</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +483,7 @@
     <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,7 +494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>41387</v>
       </c>
@@ -502,7 +505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>41388</v>
       </c>
@@ -513,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>41391</v>
       </c>
@@ -524,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>41392</v>
       </c>
@@ -534,8 +537,12 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>SUM(C2:C5)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>41394</v>
       </c>
@@ -546,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>41395</v>
       </c>
@@ -557,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>41396</v>
       </c>
@@ -568,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>41399</v>
       </c>
@@ -578,8 +585,12 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>SUM(C6:C9)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41400</v>
       </c>
@@ -590,7 +601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>41400</v>
       </c>
@@ -601,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>41403</v>
       </c>
@@ -612,7 +623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>41406</v>
       </c>
@@ -622,8 +633,12 @@
       <c r="C13" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f>SUM(C10:C13)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>41407</v>
       </c>
@@ -634,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>41409</v>
       </c>
@@ -645,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>41410</v>
       </c>
@@ -656,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>41411</v>
       </c>
@@ -666,8 +681,12 @@
       <c r="C17" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>SUM(C14:C17)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>41414</v>
       </c>
@@ -678,7 +697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41415</v>
       </c>
@@ -689,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>41418</v>
       </c>
@@ -700,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>41419</v>
       </c>
@@ -711,7 +730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41420</v>
       </c>
@@ -721,8 +740,12 @@
       <c r="C22" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>SUM(C18:C22)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41421</v>
       </c>
@@ -731,6 +754,17 @@
       </c>
       <c r="C23" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>41422</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,7 +774,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aspekt 1, Mixing E3/E4
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>diverse Projektberichte studiert für Template Projektbericht</t>
+  </si>
+  <si>
+    <t>Eclipse 4.3 Kepler + Migrationsmöglichkeiten analysiert</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,6 +802,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>41429</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
@@ -806,7 +820,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projekthandbuch Einträge Aspekt 1
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Eclipse 4.3 Kepler + Migrationsmöglichkeiten analysiert</t>
+  </si>
+  <si>
+    <t>Projekthandbuch, Statusbericht, Analyse workbench.xmi</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +816,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>41432</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1">
+        <v>8</v>
+      </c>
+    </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
@@ -820,7 +834,7 @@
       </c>
       <c r="C34" s="4">
         <f>SUM(C2:C33)</f>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zwischen Commit Projekthandbuch, bericht, etc
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Datum</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>LegacyIDE.e4xmi, Fragment und Prozessor Ansatz ausprobiert, Versionprobleme</t>
+  </si>
+  <si>
+    <t>Projekthandbuch, Statusbericht, Projektbericht</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,10 +931,23 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="3">
+        <v>41443</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="3">
+        <v>41444</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
@@ -949,7 +965,7 @@
       </c>
       <c r="C42" s="4">
         <f>SUM(C2:C41)</f>
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aktualisierter Projektbericht, Rapportierung, Planung
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Datum</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>Besprechung Betreuer, Vorbereitung Zwischenreview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nachbesprechung, Planung angepasst </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zwischenreview und Vorbereitung </t>
+  </si>
+  <si>
+    <t>Projektbericht angegangen</t>
+  </si>
+  <si>
+    <t>Handbuch, Aspekt 2 Adapters and Dependency Services, E 4.3</t>
+  </si>
+  <si>
+    <t>Handbuch, Aspekt 2 Adapters and Dependency Services, Projektbericht, E 4.3</t>
+  </si>
+  <si>
+    <t>Aktualisieren Wissen Handler / Command / Menü E4</t>
+  </si>
+  <si>
+    <t>Aktualisieren Wissen Action / Handler / Command / Menü E3</t>
   </si>
 </sst>
 </file>
@@ -515,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1030,7 @@
         <v>41453</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C41" s="1">
         <v>9</v>
@@ -1035,7 +1056,7 @@
         <v>41457</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -1046,7 +1067,7 @@
         <v>41458</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
@@ -1057,7 +1078,7 @@
         <v>41460</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C45" s="1">
         <v>8</v>
@@ -1090,16 +1111,81 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="2" t="s">
+      <c r="A48" s="3">
+        <v>41465</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>41466</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>41467</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>41468</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>41468</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <f>SUM(C47:C52)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="4">
-        <f>SUM(C2:C49)</f>
-        <v>182.5</v>
+      <c r="C57" s="4">
+        <f>SUM(C2:C52)</f>
+        <v>196.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aspekt 3 im Projekthandbuch
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Aktualisieren Wissen Action / Handler / Command / Menü E3</t>
+  </si>
+  <si>
+    <t>Handbuch, Aspekt 3 Commands / Handler, Menus, Key Bindings</t>
   </si>
 </sst>
 </file>
@@ -538,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1159,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>41468</v>
+        <v>41469</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>46</v>
@@ -1170,7 +1173,15 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="3">
+        <v>41470</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
@@ -1184,8 +1195,8 @@
         <v>6</v>
       </c>
       <c r="C57" s="4">
-        <f>SUM(C2:C52)</f>
-        <v>196.5</v>
+        <f>SUM(C2:C53)</f>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
E4 Teil Command Handlers etc. Projekthandbuch
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Datum</t>
   </si>
@@ -539,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
     <col min="3" max="3" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>41387</v>
       </c>
@@ -574,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>41388</v>
       </c>
@@ -585,7 +585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>41391</v>
       </c>
@@ -596,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>41392</v>
       </c>
@@ -610,8 +610,12 @@
         <f>SUM(C2:C5)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>D5-18</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>41394</v>
       </c>
@@ -622,7 +626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>41395</v>
       </c>
@@ -633,7 +637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>41396</v>
       </c>
@@ -644,7 +648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>41399</v>
       </c>
@@ -658,8 +662,12 @@
         <f>SUM(C6:C9)</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>D9-18</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41400</v>
       </c>
@@ -670,7 +678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>41400</v>
       </c>
@@ -681,7 +689,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>41403</v>
       </c>
@@ -692,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>41406</v>
       </c>
@@ -706,8 +714,12 @@
         <f>SUM(C10:C13)</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>D13-18</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>41407</v>
       </c>
@@ -718,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>41409</v>
       </c>
@@ -729,7 +741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>41410</v>
       </c>
@@ -740,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>41411</v>
       </c>
@@ -754,8 +766,12 @@
         <f>SUM(C14:C17)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>D17-18</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>41414</v>
       </c>
@@ -766,7 +782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41415</v>
       </c>
@@ -777,7 +793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>41418</v>
       </c>
@@ -788,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>41419</v>
       </c>
@@ -799,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41420</v>
       </c>
@@ -813,8 +829,12 @@
         <f>SUM(C18:C22)</f>
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>D22-18</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41421</v>
       </c>
@@ -825,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>41422</v>
       </c>
@@ -836,7 +856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>41426</v>
       </c>
@@ -850,8 +870,12 @@
         <f>SUM(C23:C25)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f>D25-18</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>41428</v>
       </c>
@@ -862,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>41429</v>
       </c>
@@ -873,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>41432</v>
       </c>
@@ -884,7 +908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>41433</v>
       </c>
@@ -898,8 +922,12 @@
         <f>SUM(C26:C29)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>D29-18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>41435</v>
       </c>
@@ -910,7 +938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>41436</v>
       </c>
@@ -921,7 +949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>41437</v>
       </c>
@@ -932,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>41439</v>
       </c>
@@ -943,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>41441</v>
       </c>
@@ -957,8 +985,12 @@
         <f>SUM(C30:C34)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f>D34-18</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>41442</v>
       </c>
@@ -969,7 +1001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>41443</v>
       </c>
@@ -980,7 +1012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>41444</v>
       </c>
@@ -994,8 +1026,12 @@
         <f>SUM(C35:C37)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f>D37-18</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>41449</v>
       </c>
@@ -1006,7 +1042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>41450</v>
       </c>
@@ -1017,7 +1053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>41451</v>
       </c>
@@ -1028,7 +1064,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>41453</v>
       </c>
@@ -1039,7 +1075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41455</v>
       </c>
@@ -1053,8 +1089,12 @@
         <f>SUM(C38:C42)</f>
         <v>16.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f>D42-18</f>
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41457</v>
       </c>
@@ -1065,7 +1105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>41458</v>
       </c>
@@ -1076,7 +1116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>41460</v>
       </c>
@@ -1087,7 +1127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>41461</v>
       </c>
@@ -1101,8 +1141,12 @@
         <f>SUM(C43:C46)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f>D46-18</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>41464</v>
       </c>
@@ -1113,7 +1157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>41465</v>
       </c>
@@ -1124,7 +1168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>41466</v>
       </c>
@@ -1135,7 +1179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>41467</v>
       </c>
@@ -1146,7 +1190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>41468</v>
       </c>
@@ -1157,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>41469</v>
       </c>
@@ -1171,8 +1215,12 @@
         <f>SUM(C47:C52)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <f>D52-18</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>41470</v>
       </c>
@@ -1183,7 +1231,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>41471</v>
       </c>
@@ -1194,19 +1242,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>41472</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>41473</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
finaler Commit Bericht und Handbuch
</commit_message>
<xml_diff>
--- a/Planung/Geleistete Arbeiten.xlsx
+++ b/Planung/Geleistete Arbeiten.xlsx
@@ -574,7 +574,7 @@
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
         <v>56</v>
       </c>
       <c r="C84" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1786,9 +1786,12 @@
       <c r="B85" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="C85" s="1">
+        <v>9</v>
+      </c>
       <c r="D85">
         <f>SUM(C82:C85)</f>
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +1801,7 @@
       </c>
       <c r="C86" s="3">
         <f>SUM(C2:C85)</f>
-        <v>372</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>

</xml_diff>